<commit_message>
made adjustments as per user comments
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_38_rpt_PF_JVsforFiscal-Quarter.xlsx
+++ b/backend/reports/xlsx/Tab_38_rpt_PF_JVsforFiscal-Quarter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aspiteri/Development/Github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561F916E-DE20-F74A-806D-CF673D02B971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4415811-4C5A-A24A-9305-62AB33C42F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Project #</t>
   </si>
@@ -64,9 +64,6 @@
     <t>{$r.project_number}</t>
   </si>
   <si>
-    <t>{$r1.project_number}</t>
-  </si>
-  <si>
     <t>Project JVs for Quarter {$q} Fiscal {$fy}</t>
   </si>
   <si>
@@ -80,6 +77,18 @@
   </si>
   <si>
     <t>{#fy=d.fiscal}</t>
+  </si>
+  <si>
+    <t>As of {d.current_date}</t>
+  </si>
+  <si>
+    <t>{d.report_name}</t>
+  </si>
+  <si>
+    <t>‎</t>
+  </si>
+  <si>
+    <t>{$r1}</t>
   </si>
 </sst>
 </file>
@@ -122,14 +131,14 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="0"/>
+      <b/>
+      <u/>
+      <sz val="8.5"/>
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="8.5"/>
+      <sz val="14"/>
+      <color theme="0"/>
       <name val="BCSans-Regular"/>
     </font>
   </fonts>
@@ -215,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,14 +254,20 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -276,15 +291,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>269875</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1561691</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>680356</xdr:rowOff>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>112988</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -313,8 +328,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2412591" cy="680356"/>
+          <a:off x="269875" y="47625"/>
+          <a:ext cx="1722438" cy="486051"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -614,10 +629,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -630,104 +645,133 @@
     <col min="6" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="62" customHeight="1" thickBot="1">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1" thickBot="1">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:5" ht="33" customHeight="1" thickBot="1">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" ht="23" customHeight="1" thickBot="1">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" thickBot="1">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18" customHeight="1" thickBot="1">
-      <c r="A3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9" t="s">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" ht="18" customHeight="1" thickBot="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1"/>
     <row r="7" spans="1:5" ht="18" customHeight="1">
-      <c r="B7" s="10" t="s">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" customHeight="1">
+      <c r="B8" s="10" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="19">
-      <c r="B8" s="10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="19">
       <c r="B9" s="10" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="19">
       <c r="B10" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="19">
       <c r="B11" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="19">
       <c r="B12" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19">
+      <c r="B13" s="10" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="14" spans="1:5" ht="19">
+      <c r="B14" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>